<commit_message>
Update for alt key.
</commit_message>
<xml_diff>
--- a/material/codes.xlsx
+++ b/material/codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\太田亮介\Documents\200_リポジトリ\Haidoku\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6808E540-FB41-4940-A5F6-9A42633346B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FDD663-C5B8-409A-A679-9393BA22577D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4023A06A-F075-42A2-9A9A-E49255238DA0}"/>
+    <workbookView xWindow="13815" yWindow="1830" windowWidth="24210" windowHeight="18960" xr2:uid="{4023A06A-F075-42A2-9A9A-E49255238DA0}"/>
   </bookViews>
   <sheets>
     <sheet name="codes" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="113">
   <si>
     <t>as</t>
   </si>
@@ -456,6 +456,14 @@
   </si>
   <si>
     <t>Immediately search with api when widget is displayed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ak</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>alt key view flag</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -823,7 +831,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D87C24-0B21-464C-9A96-730A23DFCF6A}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -1382,25 +1390,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" t="s">
-        <v>106</v>
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
@@ -1408,25 +1413,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" t="s">
-        <v>107</v>
+        <v>83</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
@@ -1434,10 +1436,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
         <v>49</v>
@@ -1446,13 +1448,13 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
@@ -1460,10 +1462,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
         <v>49</v>
@@ -1475,10 +1477,10 @@
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H26" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
@@ -1498,13 +1500,13 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H27" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
@@ -1512,10 +1514,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
         <v>49</v>
@@ -1527,10 +1529,10 @@
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H28" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
@@ -1538,10 +1540,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
         <v>49</v>
@@ -1553,10 +1555,10 @@
         <v>83</v>
       </c>
       <c r="G29" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
@@ -1564,10 +1566,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>49</v>
@@ -1576,13 +1578,13 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
@@ -1590,10 +1592,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
         <v>49</v>
@@ -1602,13 +1604,13 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="G31" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
@@ -1616,10 +1618,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
         <v>49</v>
@@ -1642,10 +1644,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
         <v>49</v>
@@ -1668,10 +1670,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
         <v>49</v>
@@ -1680,10 +1682,13 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="G34" t="s">
-        <v>93</v>
+        <v>46</v>
+      </c>
+      <c r="H34" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
@@ -1691,10 +1696,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
         <v>49</v>
@@ -1703,10 +1708,13 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.4">
@@ -1714,25 +1722,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>75</v>
-      </c>
-      <c r="H36" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
@@ -1740,22 +1745,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37" t="s">
-        <v>63</v>
+        <v>83</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
@@ -1778,7 +1783,10 @@
         <v>84</v>
       </c>
       <c r="G38" t="s">
-        <v>64</v>
+        <v>75</v>
+      </c>
+      <c r="H38" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
@@ -1801,7 +1809,7 @@
         <v>84</v>
       </c>
       <c r="G39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
@@ -1824,7 +1832,7 @@
         <v>84</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.4">
@@ -1847,7 +1855,7 @@
         <v>84</v>
       </c>
       <c r="G41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.4">
@@ -1870,7 +1878,7 @@
         <v>84</v>
       </c>
       <c r="G42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.4">
@@ -1878,25 +1886,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
         <v>84</v>
       </c>
       <c r="G43" t="s">
-        <v>75</v>
-      </c>
-      <c r="H43" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.4">
@@ -1904,22 +1909,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F44" t="s">
         <v>84</v>
       </c>
       <c r="G44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.4">
@@ -1942,7 +1947,10 @@
         <v>84</v>
       </c>
       <c r="G45" t="s">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="H45" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.4">
@@ -1965,7 +1973,7 @@
         <v>84</v>
       </c>
       <c r="G46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.4">
@@ -1988,7 +1996,7 @@
         <v>84</v>
       </c>
       <c r="G47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.4">
@@ -2011,7 +2019,7 @@
         <v>84</v>
       </c>
       <c r="G48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.4">
@@ -2034,7 +2042,7 @@
         <v>84</v>
       </c>
       <c r="G49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.4">
@@ -2042,22 +2050,22 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="E50">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F50" t="s">
         <v>84</v>
       </c>
       <c r="G50" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.4">
@@ -2065,22 +2073,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
       </c>
       <c r="E51">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="F51" t="s">
         <v>84</v>
       </c>
       <c r="G51" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.4">
@@ -2088,22 +2096,22 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D52" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>83</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>50</v>
+        <v>84</v>
+      </c>
+      <c r="G52" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.4">
@@ -2111,22 +2119,22 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="F53" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>51</v>
+        <v>84</v>
+      </c>
+      <c r="G53" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.4">
@@ -2134,10 +2142,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
         <v>31</v>
@@ -2157,10 +2165,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D55" t="s">
         <v>31</v>
@@ -2180,10 +2188,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D56" t="s">
         <v>31</v>
@@ -2203,10 +2211,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
         <v>31</v>
@@ -2218,6 +2226,52 @@
         <v>22</v>
       </c>
       <c r="G57" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>83</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>